<commit_message>
Atualização do arquivo1.html e arquivo1.xls
</commit_message>
<xml_diff>
--- a/arquivo1.xlsx
+++ b/arquivo1.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="13">
   <si>
     <t>Este documento foi exportado do Numbers. Cada tabela foi convertida em uma planilha do Excel. Todos os outros objetos em cada folha do Numbers foram colocados em planilhas à parte. Por favor, preste atenção porque os cálculos de fórmulas podem ser diferentes no Excel.</t>
   </si>
@@ -27,10 +27,39 @@
     <t>Nome da Planilha do Excel</t>
   </si>
   <si>
-    <t>Folha 1</t>
+    <t>Resumo da Exportação</t>
   </si>
   <si>
     <t>Tabela 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ID </t>
+  </si>
+  <si>
+    <t>Nome</t>
+  </si>
+  <si>
+    <t>Telefone</t>
+  </si>
+  <si>
+    <t>Id</t>
+  </si>
+  <si>
+    <t>Usuário da Silva</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="12"/>
+        <color indexed="11"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t>44444090</t>
+    </r>
+  </si>
+  <si>
+    <t>Folha 1</t>
   </si>
 </sst>
 </file>
@@ -40,7 +69,7 @@
   <numFmts count="1">
     <numFmt numFmtId="0" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -63,13 +92,18 @@
       <name val="Helvetica Neue"/>
     </font>
     <font>
+      <sz val="13"/>
+      <color indexed="8"/>
+      <name val="Helvetica Neue"/>
+    </font>
+    <font>
       <b val="1"/>
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Helvetica Neue"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -90,7 +124,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="12"/>
+        <fgColor indexed="13"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="14"/>
         <bgColor auto="1"/>
       </patternFill>
     </fill>
@@ -100,8 +140,20 @@
         <bgColor auto="1"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="19"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="8">
+  <borders count="20">
     <border>
       <left/>
       <right/>
@@ -111,106 +163,230 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="13"/>
+        <color indexed="12"/>
       </left>
+      <right/>
+      <top style="thin">
+        <color indexed="12"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="12"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="thin">
-        <color indexed="13"/>
+        <color indexed="12"/>
       </right>
       <top style="thin">
-        <color indexed="13"/>
+        <color indexed="12"/>
       </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="12"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="12"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="12"/>
+      </left>
+      <right/>
+      <top/>
       <bottom style="thin">
-        <color indexed="14"/>
+        <color indexed="12"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="12"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="12"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="12"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="13"/>
+        <color indexed="12"/>
       </left>
+      <right/>
+      <top style="thin">
+        <color indexed="12"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="16"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="12"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="16"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="thin">
-        <color indexed="14"/>
+        <color indexed="12"/>
       </right>
       <top style="thin">
-        <color indexed="14"/>
+        <color indexed="12"/>
       </top>
       <bottom style="thin">
-        <color indexed="13"/>
+        <color indexed="16"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="14"/>
+        <color indexed="16"/>
       </left>
       <right style="thin">
-        <color indexed="13"/>
+        <color indexed="16"/>
       </right>
       <top style="thin">
-        <color indexed="14"/>
+        <color indexed="16"/>
       </top>
       <bottom style="thin">
-        <color indexed="13"/>
+        <color indexed="18"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="13"/>
+        <color indexed="16"/>
       </left>
       <right style="thin">
-        <color indexed="13"/>
+        <color indexed="18"/>
       </right>
       <top style="thin">
-        <color indexed="14"/>
+        <color indexed="18"/>
       </top>
       <bottom style="thin">
-        <color indexed="13"/>
+        <color indexed="16"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="13"/>
+        <color indexed="18"/>
       </left>
       <right style="thin">
-        <color indexed="14"/>
+        <color indexed="16"/>
       </right>
       <top style="thin">
-        <color indexed="13"/>
+        <color indexed="18"/>
       </top>
       <bottom style="thin">
-        <color indexed="13"/>
+        <color indexed="16"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="14"/>
+        <color indexed="16"/>
       </left>
       <right style="thin">
-        <color indexed="13"/>
+        <color indexed="16"/>
       </right>
       <top style="thin">
-        <color indexed="13"/>
+        <color indexed="18"/>
       </top>
       <bottom style="thin">
-        <color indexed="13"/>
+        <color indexed="16"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="13"/>
+        <color indexed="16"/>
       </left>
       <right style="thin">
-        <color indexed="13"/>
+        <color indexed="18"/>
       </right>
       <top style="thin">
-        <color indexed="13"/>
+        <color indexed="16"/>
       </top>
       <bottom style="thin">
-        <color indexed="13"/>
+        <color indexed="16"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="18"/>
+      </left>
+      <right style="thin">
+        <color indexed="16"/>
+      </right>
+      <top style="thin">
+        <color indexed="16"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="16"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="16"/>
+      </left>
+      <right style="thin">
+        <color indexed="16"/>
+      </right>
+      <top style="thin">
+        <color indexed="16"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="16"/>
       </bottom>
       <diagonal/>
     </border>
@@ -220,7 +396,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -242,13 +418,10 @@
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -257,13 +430,82 @@
     <xf numFmtId="0" fontId="0" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="1" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="4" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="5" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="5" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="6" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="11" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="12" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="13" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="14" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="15" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="16" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="17" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="18" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="19" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -286,8 +528,12 @@
       <rgbColor rgb="015e88b1"/>
       <rgbColor rgb="01eef3f4"/>
       <rgbColor rgb="ff0000ff"/>
+      <rgbColor rgb="ffaaaaaa"/>
+      <rgbColor rgb="ff5e88b1"/>
+      <rgbColor rgb="ffeef3f4"/>
+      <rgbColor rgb="ffffffff"/>
+      <rgbColor rgb="ffa5a5a5"/>
       <rgbColor rgb="ffbdc0bf"/>
-      <rgbColor rgb="ffa5a5a5"/>
       <rgbColor rgb="ff3f3f3f"/>
       <rgbColor rgb="ffdbdbdb"/>
     </indexedColors>
@@ -306,10 +552,10 @@
         <a:srgbClr val="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="5E5E5E"/>
+        <a:srgbClr val="A7A7A7"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="D5D5D5"/>
+        <a:srgbClr val="535353"/>
       </a:lt2>
       <a:accent1>
         <a:srgbClr val="00A2FF"/>
@@ -486,11 +732,14 @@
     <a:spDef>
       <a:spPr>
         <a:solidFill>
-          <a:schemeClr val="accent1"/>
+          <a:srgbClr val="FFFFFF"/>
         </a:solidFill>
-        <a:ln w="12700" cap="flat">
-          <a:noFill/>
-          <a:miter lim="400000"/>
+        <a:ln w="25400" cap="flat">
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
@@ -499,27 +748,27 @@
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
-        <a:defPPr marL="0" marR="0" indent="0" algn="ctr" defTabSz="457200" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
-          <a:lnSpc>
-            <a:spcPct val="100000"/>
-          </a:lnSpc>
-          <a:spcBef>
-            <a:spcPts val="0"/>
-          </a:spcBef>
-          <a:spcAft>
-            <a:spcPts val="0"/>
-          </a:spcAft>
-          <a:buClrTx/>
-          <a:buSzTx/>
-          <a:buFontTx/>
-          <a:buNone/>
-          <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1200" u="none" kumimoji="0" normalizeH="0">
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:solidFill>
-              <a:srgbClr val="FFFFFF"/>
+        <a:defPPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
+          <a:lnSpc>
+            <a:spcPct val="100000"/>
+          </a:lnSpc>
+          <a:spcBef>
+            <a:spcPts val="0"/>
+          </a:spcBef>
+          <a:spcAft>
+            <a:spcPts val="0"/>
+          </a:spcAft>
+          <a:buClrTx/>
+          <a:buSzTx/>
+          <a:buFontTx/>
+          <a:buNone/>
+          <a:tabLst/>
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
@@ -776,10 +1025,10 @@
         <a:noFill/>
         <a:ln w="25400" cap="flat">
           <a:solidFill>
-            <a:srgbClr val="000000"/>
+            <a:schemeClr val="accent1"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="400000"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
@@ -1070,7 +1319,7 @@
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
-        <a:defPPr marL="0" marR="0" indent="0" algn="l" defTabSz="457200" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
+        <a:defPPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
           <a:lnSpc>
             <a:spcPct val="100000"/>
           </a:lnSpc>
@@ -1348,56 +1597,166 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10" defaultRowHeight="13" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col min="1" max="1" width="2" customWidth="1"/>
+    <col min="1" max="1" width="2" style="6" customWidth="1"/>
     <col min="2" max="4" width="33.6016" customWidth="1"/>
+    <col min="2" max="2" width="33.6719" style="6" customWidth="1"/>
+    <col min="3" max="3" width="33.6719" style="6" customWidth="1"/>
+    <col min="4" max="4" width="33.6719" style="6" customWidth="1"/>
+    <col min="5" max="5" width="10" style="6" customWidth="1"/>
+    <col min="6" max="256" width="10" style="6" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" ht="14.7" customHeight="1">
+      <c r="A1" s="7"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="9"/>
+    </row>
+    <row r="2" ht="14.7" customHeight="1">
+      <c r="A2" s="10"/>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="12"/>
+    </row>
     <row r="3" ht="50" customHeight="1">
-      <c r="B3" t="s" s="1">
+      <c r="A3" s="10"/>
+      <c r="B3" t="s" s="13">
         <v>0</v>
       </c>
-      <c r="C3"/>
-      <c r="D3"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="12"/>
+    </row>
+    <row r="4" ht="14.7" customHeight="1">
+      <c r="A4" s="10"/>
+      <c r="B4" s="11"/>
+      <c r="C4" s="11"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="12"/>
+    </row>
+    <row r="5" ht="14.7" customHeight="1">
+      <c r="A5" s="10"/>
+      <c r="B5" s="11"/>
+      <c r="C5" s="11"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="12"/>
+    </row>
+    <row r="6" ht="14.7" customHeight="1">
+      <c r="A6" s="10"/>
+      <c r="B6" s="11"/>
+      <c r="C6" s="11"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="12"/>
     </row>
     <row r="7">
-      <c r="B7" t="s" s="2">
+      <c r="A7" s="10"/>
+      <c r="B7" t="s" s="14">
+        <v>6</v>
+      </c>
+      <c r="C7" t="s" s="14">
+        <v>7</v>
+      </c>
+      <c r="D7" t="s" s="14">
+        <v>8</v>
+      </c>
+      <c r="E7" s="12"/>
+    </row>
+    <row r="8" ht="14.7" customHeight="1">
+      <c r="A8" s="10"/>
+      <c r="B8" s="11"/>
+      <c r="C8" s="11"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="12"/>
+    </row>
+    <row r="9">
+      <c r="A9" s="10"/>
+      <c r="B9" t="s" s="15">
+        <v>9</v>
+      </c>
+      <c r="C9" s="16"/>
+      <c r="D9" s="16"/>
+      <c r="E9" s="12"/>
+    </row>
+    <row r="10">
+      <c r="A10" s="10"/>
+      <c r="B10" s="17">
         <v>1</v>
       </c>
-      <c r="C7" t="s" s="2">
-        <v>2</v>
+      <c r="C10" t="s" s="18">
+        <v>10</v>
       </c>
-      <c r="D7" t="s" s="2">
-        <v>3</v>
+      <c r="D10" t="s" s="19">
+        <v>11</v>
       </c>
-    </row>
-    <row r="9">
-      <c r="B9" t="s" s="3">
-        <v>4</v>
+      <c r="E10" s="12"/>
+    </row>
+    <row r="11" ht="13" customHeight="1">
+      <c r="A11" s="10"/>
+      <c r="B11" t="s" s="3">
+        <v>12</v>
       </c>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-    </row>
-    <row r="10">
-      <c r="B10" s="4"/>
-      <c r="C10" t="s" s="4">
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="12"/>
+    </row>
+    <row r="12" ht="13" customHeight="1">
+      <c r="A12" s="10"/>
+      <c r="B12" s="4"/>
+      <c r="C12" t="s" s="4">
         <v>5</v>
       </c>
-      <c r="D10" t="s" s="5">
-        <v>4</v>
+      <c r="D12" t="s" s="5">
+        <v>12</v>
       </c>
+      <c r="E12" s="12"/>
+    </row>
+    <row r="13" ht="16.65" customHeight="1">
+      <c r="A13" s="10"/>
+      <c r="B13" s="20"/>
+      <c r="C13" s="20"/>
+      <c r="D13" s="21"/>
+      <c r="E13" s="12"/>
+    </row>
+    <row r="14" ht="16.65" customHeight="1">
+      <c r="A14" s="10"/>
+      <c r="B14" s="20"/>
+      <c r="C14" s="20"/>
+      <c r="D14" s="21"/>
+      <c r="E14" s="12"/>
+    </row>
+    <row r="15" ht="16.65" customHeight="1">
+      <c r="A15" s="22"/>
+      <c r="B15" s="23"/>
+      <c r="C15" s="23"/>
+      <c r="D15" s="24"/>
+      <c r="E15" s="25"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
+    <mergeCell ref="B3:D3"/>
     <mergeCell ref="B3:D3"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="D10" location="'Folha 1'!R2C1" tooltip="" display="Folha 1"/>
+    <hyperlink ref="D10" location="'Resumo da Exportação'!R1C1" tooltip="" display="Resumo da Exportação"/>
+    <hyperlink ref="D12" location="'Folha 1'!R1C1" tooltip="" display="Folha 1"/>
   </hyperlinks>
+  <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
+  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <headerFooter>
+    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
 
@@ -1406,226 +1765,224 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A2:G23"/>
+  <dimension ref="A1:G23"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1">
-      <pane topLeftCell="B3" xSplit="1" ySplit="2" activePane="bottomRight" state="frozen"/>
-    </sheetView>
+    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="19.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="7" width="16.3516" style="6" customWidth="1"/>
-    <col min="8" max="256" width="16.3516" style="6" customWidth="1"/>
+    <col min="1" max="7" width="16.3516" style="26" customWidth="1"/>
+    <col min="8" max="256" width="16.3516" style="26" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="27.65" customHeight="1">
-      <c r="A1" t="s" s="7">
+      <c r="A1" t="s" s="27">
         <v>5</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="29"/>
     </row>
     <row r="2" ht="20.25" customHeight="1">
-      <c r="A2" s="8"/>
-      <c r="B2" s="8"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8"/>
+      <c r="A2" s="30"/>
+      <c r="B2" s="30"/>
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="30"/>
+      <c r="F2" s="30"/>
+      <c r="G2" s="30"/>
     </row>
     <row r="3" ht="20.25" customHeight="1">
-      <c r="A3" s="9"/>
-      <c r="B3" s="10"/>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="11"/>
-      <c r="F3" s="11"/>
-      <c r="G3" s="11"/>
+      <c r="A3" s="31"/>
+      <c r="B3" s="32"/>
+      <c r="C3" s="33"/>
+      <c r="D3" s="33"/>
+      <c r="E3" s="33"/>
+      <c r="F3" s="33"/>
+      <c r="G3" s="33"/>
     </row>
     <row r="4" ht="20.05" customHeight="1">
-      <c r="A4" s="12"/>
-      <c r="B4" s="13"/>
-      <c r="C4" s="14"/>
-      <c r="D4" s="14"/>
-      <c r="E4" s="14"/>
-      <c r="F4" s="14"/>
-      <c r="G4" s="14"/>
+      <c r="A4" s="34"/>
+      <c r="B4" s="35"/>
+      <c r="C4" s="36"/>
+      <c r="D4" s="36"/>
+      <c r="E4" s="36"/>
+      <c r="F4" s="36"/>
+      <c r="G4" s="36"/>
     </row>
     <row r="5" ht="20.05" customHeight="1">
-      <c r="A5" s="12"/>
-      <c r="B5" s="13"/>
-      <c r="C5" s="14"/>
-      <c r="D5" s="14"/>
-      <c r="E5" s="14"/>
-      <c r="F5" s="14"/>
-      <c r="G5" s="14"/>
+      <c r="A5" s="34"/>
+      <c r="B5" s="35"/>
+      <c r="C5" s="36"/>
+      <c r="D5" s="36"/>
+      <c r="E5" s="36"/>
+      <c r="F5" s="36"/>
+      <c r="G5" s="36"/>
     </row>
     <row r="6" ht="20.05" customHeight="1">
-      <c r="A6" s="12"/>
-      <c r="B6" s="13"/>
-      <c r="C6" s="14"/>
-      <c r="D6" s="14"/>
-      <c r="E6" s="14"/>
-      <c r="F6" s="14"/>
-      <c r="G6" s="14"/>
+      <c r="A6" s="34"/>
+      <c r="B6" s="35"/>
+      <c r="C6" s="36"/>
+      <c r="D6" s="36"/>
+      <c r="E6" s="36"/>
+      <c r="F6" s="36"/>
+      <c r="G6" s="36"/>
     </row>
     <row r="7" ht="20.05" customHeight="1">
-      <c r="A7" s="12"/>
-      <c r="B7" s="13"/>
-      <c r="C7" s="14"/>
-      <c r="D7" s="14"/>
-      <c r="E7" s="14"/>
-      <c r="F7" s="14"/>
-      <c r="G7" s="14"/>
+      <c r="A7" s="34"/>
+      <c r="B7" s="35"/>
+      <c r="C7" s="36"/>
+      <c r="D7" s="36"/>
+      <c r="E7" s="36"/>
+      <c r="F7" s="36"/>
+      <c r="G7" s="36"/>
     </row>
     <row r="8" ht="20.05" customHeight="1">
-      <c r="A8" s="12"/>
-      <c r="B8" s="13"/>
-      <c r="C8" s="14"/>
-      <c r="D8" s="14"/>
-      <c r="E8" s="14"/>
-      <c r="F8" s="14"/>
-      <c r="G8" s="14"/>
+      <c r="A8" s="34"/>
+      <c r="B8" s="35"/>
+      <c r="C8" s="36"/>
+      <c r="D8" s="36"/>
+      <c r="E8" s="36"/>
+      <c r="F8" s="36"/>
+      <c r="G8" s="36"/>
     </row>
     <row r="9" ht="20.05" customHeight="1">
-      <c r="A9" s="12"/>
-      <c r="B9" s="13"/>
-      <c r="C9" s="14"/>
-      <c r="D9" s="14"/>
-      <c r="E9" s="14"/>
-      <c r="F9" s="14"/>
-      <c r="G9" s="14"/>
+      <c r="A9" s="34"/>
+      <c r="B9" s="35"/>
+      <c r="C9" s="36"/>
+      <c r="D9" s="36"/>
+      <c r="E9" s="36"/>
+      <c r="F9" s="36"/>
+      <c r="G9" s="36"/>
     </row>
     <row r="10" ht="20.05" customHeight="1">
-      <c r="A10" s="12"/>
-      <c r="B10" s="13"/>
-      <c r="C10" s="14"/>
-      <c r="D10" s="14"/>
-      <c r="E10" s="14"/>
-      <c r="F10" s="14"/>
-      <c r="G10" s="14"/>
+      <c r="A10" s="34"/>
+      <c r="B10" s="35"/>
+      <c r="C10" s="36"/>
+      <c r="D10" s="36"/>
+      <c r="E10" s="36"/>
+      <c r="F10" s="36"/>
+      <c r="G10" s="36"/>
     </row>
     <row r="11" ht="20.05" customHeight="1">
-      <c r="A11" s="12"/>
-      <c r="B11" s="13"/>
-      <c r="C11" s="14"/>
-      <c r="D11" s="14"/>
-      <c r="E11" s="14"/>
-      <c r="F11" s="14"/>
-      <c r="G11" s="14"/>
+      <c r="A11" s="34"/>
+      <c r="B11" s="35"/>
+      <c r="C11" s="36"/>
+      <c r="D11" s="36"/>
+      <c r="E11" s="36"/>
+      <c r="F11" s="36"/>
+      <c r="G11" s="36"/>
     </row>
     <row r="12" ht="20.05" customHeight="1">
-      <c r="A12" s="12"/>
-      <c r="B12" s="13"/>
-      <c r="C12" s="14"/>
-      <c r="D12" s="14"/>
-      <c r="E12" s="14"/>
-      <c r="F12" s="14"/>
-      <c r="G12" s="14"/>
+      <c r="A12" s="34"/>
+      <c r="B12" s="35"/>
+      <c r="C12" s="36"/>
+      <c r="D12" s="36"/>
+      <c r="E12" s="36"/>
+      <c r="F12" s="36"/>
+      <c r="G12" s="36"/>
     </row>
     <row r="13" ht="20.05" customHeight="1">
-      <c r="A13" s="12"/>
-      <c r="B13" s="13"/>
-      <c r="C13" s="14"/>
-      <c r="D13" s="14"/>
-      <c r="E13" s="14"/>
-      <c r="F13" s="14"/>
-      <c r="G13" s="14"/>
+      <c r="A13" s="34"/>
+      <c r="B13" s="35"/>
+      <c r="C13" s="36"/>
+      <c r="D13" s="36"/>
+      <c r="E13" s="36"/>
+      <c r="F13" s="36"/>
+      <c r="G13" s="36"/>
     </row>
     <row r="14" ht="20.05" customHeight="1">
-      <c r="A14" s="12"/>
-      <c r="B14" s="13"/>
-      <c r="C14" s="14"/>
-      <c r="D14" s="14"/>
-      <c r="E14" s="14"/>
-      <c r="F14" s="14"/>
-      <c r="G14" s="14"/>
+      <c r="A14" s="34"/>
+      <c r="B14" s="35"/>
+      <c r="C14" s="36"/>
+      <c r="D14" s="36"/>
+      <c r="E14" s="36"/>
+      <c r="F14" s="36"/>
+      <c r="G14" s="36"/>
     </row>
     <row r="15" ht="20.05" customHeight="1">
-      <c r="A15" s="12"/>
-      <c r="B15" s="13"/>
-      <c r="C15" s="14"/>
-      <c r="D15" s="14"/>
-      <c r="E15" s="14"/>
-      <c r="F15" s="14"/>
-      <c r="G15" s="14"/>
+      <c r="A15" s="34"/>
+      <c r="B15" s="35"/>
+      <c r="C15" s="36"/>
+      <c r="D15" s="36"/>
+      <c r="E15" s="36"/>
+      <c r="F15" s="36"/>
+      <c r="G15" s="36"/>
     </row>
     <row r="16" ht="20.05" customHeight="1">
-      <c r="A16" s="12"/>
-      <c r="B16" s="13"/>
-      <c r="C16" s="14"/>
-      <c r="D16" s="14"/>
-      <c r="E16" s="14"/>
-      <c r="F16" s="14"/>
-      <c r="G16" s="14"/>
+      <c r="A16" s="34"/>
+      <c r="B16" s="35"/>
+      <c r="C16" s="36"/>
+      <c r="D16" s="36"/>
+      <c r="E16" s="36"/>
+      <c r="F16" s="36"/>
+      <c r="G16" s="36"/>
     </row>
     <row r="17" ht="20.05" customHeight="1">
-      <c r="A17" s="12"/>
-      <c r="B17" s="13"/>
-      <c r="C17" s="14"/>
-      <c r="D17" s="14"/>
-      <c r="E17" s="14"/>
-      <c r="F17" s="14"/>
-      <c r="G17" s="14"/>
+      <c r="A17" s="34"/>
+      <c r="B17" s="35"/>
+      <c r="C17" s="36"/>
+      <c r="D17" s="36"/>
+      <c r="E17" s="36"/>
+      <c r="F17" s="36"/>
+      <c r="G17" s="36"/>
     </row>
     <row r="18" ht="20.05" customHeight="1">
-      <c r="A18" s="12"/>
-      <c r="B18" s="13"/>
-      <c r="C18" s="14"/>
-      <c r="D18" s="14"/>
-      <c r="E18" s="14"/>
-      <c r="F18" s="14"/>
-      <c r="G18" s="14"/>
+      <c r="A18" s="34"/>
+      <c r="B18" s="35"/>
+      <c r="C18" s="36"/>
+      <c r="D18" s="36"/>
+      <c r="E18" s="36"/>
+      <c r="F18" s="36"/>
+      <c r="G18" s="36"/>
     </row>
     <row r="19" ht="20.05" customHeight="1">
-      <c r="A19" s="12"/>
-      <c r="B19" s="13"/>
-      <c r="C19" s="14"/>
-      <c r="D19" s="14"/>
-      <c r="E19" s="14"/>
-      <c r="F19" s="14"/>
-      <c r="G19" s="14"/>
+      <c r="A19" s="34"/>
+      <c r="B19" s="35"/>
+      <c r="C19" s="36"/>
+      <c r="D19" s="36"/>
+      <c r="E19" s="36"/>
+      <c r="F19" s="36"/>
+      <c r="G19" s="36"/>
     </row>
     <row r="20" ht="20.05" customHeight="1">
-      <c r="A20" s="12"/>
-      <c r="B20" s="13"/>
-      <c r="C20" s="14"/>
-      <c r="D20" s="14"/>
-      <c r="E20" s="14"/>
-      <c r="F20" s="14"/>
-      <c r="G20" s="14"/>
+      <c r="A20" s="34"/>
+      <c r="B20" s="35"/>
+      <c r="C20" s="36"/>
+      <c r="D20" s="36"/>
+      <c r="E20" s="36"/>
+      <c r="F20" s="36"/>
+      <c r="G20" s="36"/>
     </row>
     <row r="21" ht="20.05" customHeight="1">
-      <c r="A21" s="12"/>
-      <c r="B21" s="13"/>
-      <c r="C21" s="14"/>
-      <c r="D21" s="14"/>
-      <c r="E21" s="14"/>
-      <c r="F21" s="14"/>
-      <c r="G21" s="14"/>
+      <c r="A21" s="34"/>
+      <c r="B21" s="35"/>
+      <c r="C21" s="36"/>
+      <c r="D21" s="36"/>
+      <c r="E21" s="36"/>
+      <c r="F21" s="36"/>
+      <c r="G21" s="36"/>
     </row>
     <row r="22" ht="20.05" customHeight="1">
-      <c r="A22" s="12"/>
-      <c r="B22" s="13"/>
-      <c r="C22" s="14"/>
-      <c r="D22" s="14"/>
-      <c r="E22" s="14"/>
-      <c r="F22" s="14"/>
-      <c r="G22" s="14"/>
+      <c r="A22" s="34"/>
+      <c r="B22" s="35"/>
+      <c r="C22" s="36"/>
+      <c r="D22" s="36"/>
+      <c r="E22" s="36"/>
+      <c r="F22" s="36"/>
+      <c r="G22" s="36"/>
     </row>
     <row r="23" ht="20.05" customHeight="1">
-      <c r="A23" s="12"/>
-      <c r="B23" s="13"/>
-      <c r="C23" s="14"/>
-      <c r="D23" s="14"/>
-      <c r="E23" s="14"/>
-      <c r="F23" s="14"/>
-      <c r="G23" s="14"/>
+      <c r="A23" s="34"/>
+      <c r="B23" s="35"/>
+      <c r="C23" s="36"/>
+      <c r="D23" s="36"/>
+      <c r="E23" s="36"/>
+      <c r="F23" s="36"/>
+      <c r="G23" s="36"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>